<commit_message>
adde protection to the excel
</commit_message>
<xml_diff>
--- a/State Wise Covid Analyis.xlsx
+++ b/State Wise Covid Analyis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joker\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joker\Desktop\JobHunt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D3B225-79B1-4167-937D-50843D90D6BE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A528B0B5-71CD-442B-A4EA-1B797829B360}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{06ACA2B7-BA38-4BC2-8DF7-00EE78D5992F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
   <si>
     <t>S. No.</t>
   </si>
@@ -336,6 +336,9 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -372,9 +375,6 @@
           <color rgb="FF3F3F3F"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -467,63 +467,7 @@
           </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:tint val="100000"/>
-                    <a:shade val="85000"/>
-                    <a:satMod val="100000"/>
-                    <a:lumMod val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:tint val="90000"/>
-                    <a:shade val="100000"/>
-                    <a:satMod val="150000"/>
-                    <a:lumMod val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="100000" t="100000" r="100000" b="100000"/>
-              </a:path>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="76200" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="60000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-            <a:scene3d>
-              <a:camera prst="orthographicFront">
-                <a:rot lat="0" lon="0" rev="0"/>
-              </a:camera>
-              <a:lightRig rig="flat" dir="t">
-                <a:rot lat="0" lon="0" rev="3600000"/>
-              </a:lightRig>
-            </a:scene3d>
-            <a:sp3d contourW="12700" prstMaterial="flat">
-              <a:bevelT w="38100" h="44450" prst="angle"/>
-              <a:contourClr>
-                <a:scrgbClr r="0" g="0" b="0">
-                  <a:shade val="35000"/>
-                  <a:satMod val="160000"/>
-                </a:scrgbClr>
-              </a:contourClr>
-            </a:sp3d>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2406,8 +2350,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Name of State / UT">
@@ -2430,7 +2374,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2839,7 +2783,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D330A77C-9FE8-4649-AA1E-B2F7E663BB48}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D330A77C-9FE8-4649-AA1E-B2F7E663BB48}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A4:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -3135,10 +3079,10 @@
     <tableColumn id="4" xr3:uid="{FE5CF12B-F288-489D-8EA3-E3BC1ADE02EC}" name="Total Confirmed cases ( Foreign National )" totalsRowFunction="count"/>
     <tableColumn id="5" xr3:uid="{82CC0C3F-C522-466C-A5FD-6B772335A193}" name="Cured" totalsRowFunction="count"/>
     <tableColumn id="6" xr3:uid="{1D4E977B-1B8A-4ADF-8D12-E6793579883B}" name="Death" totalsRowFunction="count"/>
-    <tableColumn id="7" xr3:uid="{93D3F185-5E2E-4BB7-9063-BD1E9323DA91}" name="Active cases" totalsRowFunction="count" dataDxfId="3" totalsRowDxfId="1" dataCellStyle="Output">
+    <tableColumn id="7" xr3:uid="{93D3F185-5E2E-4BB7-9063-BD1E9323DA91}" name="Active cases" totalsRowFunction="count" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Output">
       <calculatedColumnFormula>Tbl_Corona[[#This Row],[Total]]-Tbl_Corona[[#This Row],[Cured]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AD07C3DD-1BEB-4D5E-B107-1203C3D15309}" name="Total" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="0" dataCellStyle="Output">
+    <tableColumn id="8" xr3:uid="{AD07C3DD-1BEB-4D5E-B107-1203C3D15309}" name="Total" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Output">
       <calculatedColumnFormula>Tbl_Corona[[#This Row],[Total Confirmed cases (Indian National)]]+Tbl_Corona[[#This Row],[Total Confirmed cases ( Foreign National )]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4080,7 +4024,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DC7810-D3D1-4CDC-97EB-375323C7B68B}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4789,6 +4735,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <conditionalFormatting sqref="G29:G1048576 G1">
     <cfRule type="dataBar" priority="2">
       <dataBar>
@@ -4863,7 +4810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E22BD2-080D-4026-8642-8408B6E38087}">
   <dimension ref="A3:A29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5114,6 +5063,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
   <extLst>

</xml_diff>